<commit_message>
rename *validate_model* methods to *check_model* methods, and inconsistencies to uninitialized_attrs; fully test migrate_over_schema_sequence
</commit_message>
<xml_diff>
--- a/tests/fixtures/migrate/example_old_model_rt.xlsx
+++ b/tests/fixtures/migrate/example_old_model_rt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25140" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25140" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Id</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Karr et al., 2016 Mycoplasma pneumoniae M129 model</t>
   </si>
   <si>
     <t>Version</t>
@@ -448,6 +445,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
@@ -465,81 +521,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="15" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -571,32 +566,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -626,15 +621,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>